<commit_message>
fix pivot on dynamic sheet
</commit_message>
<xml_diff>
--- a/samples/src/test/resources/samples/PivotReport.xlsx
+++ b/samples/src/test/resources/samples/PivotReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,7 +10,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Total</t>
   </si>
@@ -55,15 +55,12 @@
   <si>
     <t>Sum of Premium</t>
   </si>
-  <si>
-    <t>#eval 0</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,10 +105,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -146,6 +143,11 @@
       <sharedItems/>
     </cacheField>
   </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
 </pivotCacheDefinition>
 </file>
 
@@ -290,6 +292,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -324,6 +327,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,26 +503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -526,7 +525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -534,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -548,19 +547,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -574,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -588,13 +587,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="2">
-        <f>SUBTOTAL(109,[Premium])</f>
+        <f>SUBTOTAL(109,Table1[Premium])</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>